<commit_message>
corrigindo erro de zip file
</commit_message>
<xml_diff>
--- a/src/output_test/test_data/controle-de-arquivos-tjrr-2019-09.xlsx
+++ b/src/output_test/test_data/controle-de-arquivos-tjrr-2019-09.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -380,18 +380,18 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>